<commit_message>
added json file, need to setup the index page and js script page
</commit_message>
<xml_diff>
--- a/last.xlsx
+++ b/last.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manisha.patel/Project/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAD432E1-4F8D-0A40-B0B8-0B295F3544F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C173130-4053-8F48-997C-344AA6B7EA8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14220"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14740"/>
   </bookViews>
   <sheets>
-    <sheet name="file020719" sheetId="1" r:id="rId1"/>
+    <sheet name="last" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -616,25 +616,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>file020719!$A$1</c:f>
+              <c:f>last!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>range</c:v>
+                  <c:v>time_taken</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -643,14 +643,26 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>file020719!$A$2:$A$21</c:f>
+              <c:f>last!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -710,110 +722,77 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>last!$B$2:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2.99999737762846E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9999977161642099E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.00000033853575E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.00000033853575E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0000006770715101E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.00000101560726E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9999977161642099E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.00000101560726E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.99999737762846E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.00000033853575E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0000006770715101E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9999970390927E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0000006770715101E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9999970390927E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.0000013541430202E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.99999737762846E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0000006770715101E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9999970390927E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0000013541430202E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-007C-FD4F-BBC5-ED0E690F9C6A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>file020719!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>time_taken</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>file020719!$B$2:$B$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-007C-FD4F-BBC5-ED0E690F9C6A}"/>
+              <c16:uniqueId val="{00000000-F0FD-1C40-BB7E-681E69F64E52}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -825,17 +804,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="402601103"/>
-        <c:axId val="460275823"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="402601103"/>
+        <c:axId val="529326095"/>
+        <c:axId val="529327775"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="529326095"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -844,8 +837,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -872,15 +865,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="460275823"/>
+        <c:crossAx val="529327775"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="460275823"/>
+        <c:axId val="529327775"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,8 +896,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -931,9 +927,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="402601103"/>
+        <c:crossAx val="529326095"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -943,37 +939,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1059,7 +1024,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1086,8 +1051,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1167,11 +1132,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1182,11 +1142,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1198,7 +1153,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1218,9 +1173,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1233,10 +1185,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1276,22 +1228,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1396,8 +1349,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1529,19 +1482,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1555,6 +1509,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1578,23 +1543,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F81A781F-6AC6-1A40-A0D6-E1EC7C8C6D3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A3ED864-CDB5-CC41-9CD7-73A63776830D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1914,9 +1879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1933,7 +1896,7 @@
         <v>5000</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>2.99999737762846E-4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1941,7 +1904,7 @@
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>3.9999977161642099E-4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1949,7 +1912,7 @@
         <v>15000</v>
       </c>
       <c r="B4">
-        <v>1000</v>
+        <v>1.00000033853575E-4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1957,7 +1920,7 @@
         <v>20000</v>
       </c>
       <c r="B5">
-        <v>1000</v>
+        <v>1.00000033853575E-4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1965,7 +1928,7 @@
         <v>25000</v>
       </c>
       <c r="B6">
-        <v>1000</v>
+        <v>2.0000006770715101E-4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1973,7 +1936,7 @@
         <v>30000</v>
       </c>
       <c r="B7">
-        <v>1000</v>
+        <v>3.00000101560726E-4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1981,7 +1944,7 @@
         <v>35000</v>
       </c>
       <c r="B8">
-        <v>1000</v>
+        <v>3.9999977161642099E-4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1989,7 +1952,7 @@
         <v>40000</v>
       </c>
       <c r="B9">
-        <v>1000</v>
+        <v>3.00000101560726E-4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1997,7 +1960,7 @@
         <v>45000</v>
       </c>
       <c r="B10">
-        <v>1000</v>
+        <v>2.99999737762846E-4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2005,7 +1968,7 @@
         <v>50000</v>
       </c>
       <c r="B11">
-        <v>1000</v>
+        <v>1.00000033853575E-4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2013,7 +1976,7 @@
         <v>55000</v>
       </c>
       <c r="B12">
-        <v>1000</v>
+        <v>2.0000006770715101E-4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2021,7 +1984,7 @@
         <v>60000</v>
       </c>
       <c r="B13">
-        <v>1000</v>
+        <v>1.9999970390927E-4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2029,7 +1992,7 @@
         <v>65000</v>
       </c>
       <c r="B14">
-        <v>1000</v>
+        <v>2.0000006770715101E-4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2037,7 +2000,7 @@
         <v>70000</v>
       </c>
       <c r="B15">
-        <v>1000</v>
+        <v>1.9999970390927E-4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2045,7 +2008,7 @@
         <v>75000</v>
       </c>
       <c r="B16">
-        <v>1000</v>
+        <v>4.0000013541430202E-4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2053,7 +2016,7 @@
         <v>80000</v>
       </c>
       <c r="B17">
-        <v>1000</v>
+        <v>2.99999737762846E-4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2061,7 +2024,7 @@
         <v>85000</v>
       </c>
       <c r="B18">
-        <v>1000</v>
+        <v>2.0000006770715101E-4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2069,7 +2032,7 @@
         <v>90000</v>
       </c>
       <c r="B19">
-        <v>1000</v>
+        <v>1.9999970390927E-4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2077,7 +2040,7 @@
         <v>95000</v>
       </c>
       <c r="B20">
-        <v>1000</v>
+        <v>4.0000013541430202E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>